<commit_message>
Amplifier testing procedure started - initial test to make sure it works - beginning to test for real world electrical/mechanical conditions
</commit_message>
<xml_diff>
--- a/Revision01/Testing/dataForAmplifierTestingProcedure.xlsx
+++ b/Revision01/Testing/dataForAmplifierTestingProcedure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parry\Documents\GitHub\BCIT-BAJA-DAQ\Revision01\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parry\Documents\GITHUB_desktop\BCIT-BAJA-DAQ\Revision01\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{294E18E1-0CD7-440C-821D-FD41B55D56E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A459915-5C97-41F0-A31E-A1C7277EC454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3EB0B6A-98A8-484E-8743-3616FB1D4677}"/>
+    <workbookView xWindow="-30816" yWindow="-96" windowWidth="30912" windowHeight="16752" xr2:uid="{F3EB0B6A-98A8-484E-8743-3616FB1D4677}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Offset voltage</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>resolution</t>
+  </si>
+  <si>
+    <t>magnitude and phase response</t>
+  </si>
+  <si>
+    <t>StrainDifferential(mV)</t>
+  </si>
+  <si>
+    <t>100Hz sin wave (-10mV,10mV)</t>
   </si>
 </sst>
 </file>
@@ -431,40 +440,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E5EB1D-674F-491E-A6E7-628378061F24}">
-  <dimension ref="A5:A9"/>
+  <dimension ref="A5:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>